<commit_message>
adding a review log for DIO_TEST
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Review No.</t>
   </si>
@@ -148,13 +148,31 @@
   </si>
   <si>
     <t>walaa</t>
+  </si>
+  <si>
+    <t>Reviewed by</t>
+  </si>
+  <si>
+    <t>anwar abd elhamid</t>
+  </si>
+  <si>
+    <t>rev-09</t>
+  </si>
+  <si>
+    <t>DIO_TEST</t>
+  </si>
+  <si>
+    <t>more test scenarios needed for each funtion</t>
+  </si>
+  <si>
+    <t>abdel azim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +180,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +231,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,28 +246,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -244,12 +308,54 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -257,19 +363,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -291,13 +394,13 @@
     <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="Review No." dataDxfId="5"/>
-    <tableColumn id="2" name="Document Name" dataDxfId="3"/>
+    <tableColumn id="1" name="Review No." dataDxfId="6"/>
+    <tableColumn id="2" name="Document Name" dataDxfId="5"/>
     <tableColumn id="4" name="Changes" dataDxfId="4"/>
-    <tableColumn id="7" name="date reviewed" dataDxfId="6"/>
+    <tableColumn id="7" name="date reviewed" dataDxfId="3"/>
     <tableColumn id="5" name="Complexity" dataDxfId="2"/>
-    <tableColumn id="6" name="assigned person" dataDxfId="0"/>
-    <tableColumn id="3" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="assigned person" dataDxfId="1"/>
+    <tableColumn id="3" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -588,247 +691,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="5" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45">
-      <c r="A2" s="3" t="s">
+      <c r="H1" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45">
+      <c r="A2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30">
-      <c r="A3" s="3" t="s">
+      <c r="H2" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="20" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="48.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="H3" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="48.75" customHeight="1">
+      <c r="A4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
+      <c r="H4" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="H6" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32.25" customHeight="1">
+      <c r="A7" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="64.5" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="H7" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="64.5" customHeight="1">
+      <c r="A8" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>42373</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="33" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="H8" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="33" customHeight="1">
+      <c r="A9" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <v>42373</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="H9" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="27.75" customHeight="1">
+      <c r="A10" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="14">
         <v>42373</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="15"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="15"/>
+      <c r="H10" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="52.5" customHeight="1">
+      <c r="A11" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="21">
+        <v>42555</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="13"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="13"/>
+      <c r="H19" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding rev-10 in review log
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Review No.</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>abdel azim</t>
+  </si>
+  <si>
+    <t>rev-10</t>
+  </si>
+  <si>
+    <t>testcases column needs to be renamed to function ID.</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +240,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,6 +359,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,7 +715,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,8 +1003,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="H12" s="16"/>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="21">
+        <v>42586</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="H13" s="16"/>

</xml_diff>

<commit_message>
updating the review log with rev-11
rev-11 related to the SWITCH_TEST
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Review No.</t>
   </si>
@@ -172,13 +172,25 @@
   </si>
   <si>
     <t>testcases column needs to be renamed to function ID.</t>
+  </si>
+  <si>
+    <t>rev-11</t>
+  </si>
+  <si>
+    <t>SWITCH_TEST</t>
+  </si>
+  <si>
+    <t>test scnearios are too few ,more unhappy scenarios needed</t>
+  </si>
+  <si>
+    <t>seif eldin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +225,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,6 +387,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,7 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +803,7 @@
       <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="31" t="s">
         <v>45</v>
       </c>
     </row>
@@ -804,7 +829,7 @@
       <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="31" t="s">
         <v>45</v>
       </c>
     </row>
@@ -830,7 +855,7 @@
       <c r="G4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="31" t="s">
         <v>45</v>
       </c>
     </row>
@@ -845,7 +870,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="17"/>
       <c r="F5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" s="26" t="s">
@@ -869,7 +894,7 @@
       <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -895,7 +920,7 @@
       <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -921,7 +946,7 @@
       <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -947,7 +972,7 @@
       <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -973,7 +998,7 @@
       <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -999,7 +1024,7 @@
       <c r="G11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1007,7 +1032,7 @@
       <c r="A12" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="23" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="28" t="s">
@@ -1019,18 +1044,41 @@
       <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="16" t="s">
         <v>49</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="H13" s="16"/>
+    <row r="13" spans="1:8" ht="45">
+      <c r="A13" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="21">
+        <v>42586</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="H14" s="16"/>

</xml_diff>

<commit_message>
adding rev-12 to review log related to the intergation testing
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/Review-Log-Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>Review No.</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>seif eldin</t>
+  </si>
+  <si>
+    <t>rev-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration Test </t>
+  </si>
+  <si>
+    <t>bad test scenarios. More scenarios needed with each two modules</t>
   </si>
 </sst>
 </file>
@@ -740,7 +749,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1047,8 +1056,8 @@
       <c r="F12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="30" t="s">
-        <v>32</v>
+      <c r="G12" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="H12" s="31" t="s">
         <v>31</v>
@@ -1080,8 +1089,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="H14" s="16"/>
+    <row r="14" spans="1:8" ht="45">
+      <c r="A14" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="21">
+        <v>42586</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="H15" s="16"/>

</xml_diff>